<commit_message>
introducing the test plan spreadsheet
</commit_message>
<xml_diff>
--- a/test/TestPlan.xlsx
+++ b/test/TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>Given</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Log In</t>
+  </si>
+  <si>
+    <t>User_ChangePassword</t>
   </si>
 </sst>
 </file>
@@ -803,8 +806,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,6 +1380,15 @@
       </c>
       <c r="D55" s="4" t="s">
         <v>68</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">

</xml_diff>